<commit_message>
added xlsx file with session
</commit_message>
<xml_diff>
--- a/resources/whist.xlsx
+++ b/resources/whist.xlsx
@@ -482,7 +482,7 @@
   <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="70" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G70">
-        <f t="shared" ref="G24:G71" si="1">SUM(C71:F71)</f>
+        <f t="shared" ref="G70:G71" si="1">SUM(C71:F71)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>